<commit_message>
Add matlab script to plot sediment data. Upload sediment data.
</commit_message>
<xml_diff>
--- a/data/20220919_sediment_data/Sediment_CB_09192022.xlsx
+++ b/data/20220919_sediment_data/Sediment_CB_09192022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CLASSES_2021_2022\Fall_2022\EGN_495\capstone\sediment_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CLASSES_2021_2022\Fall_2022\EGN_495\capstone\data\20220919_sediment_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86629FBA-7578-4FDE-BA2F-8AE38531D4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592BE0C8-FF8C-4783-968F-36CB4383B7CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="681" xr2:uid="{DE57CDD9-9D95-44F8-A719-10E7657C7FAC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="670" xr2:uid="{DE57CDD9-9D95-44F8-A719-10E7657C7FAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="40">
   <si>
     <t>Transect ID</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Negative percent loss doesn't make sense. We gained sediment?</t>
   </si>
 </sst>
 </file>
@@ -726,7 +723,7 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,9 +789,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="28" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="30" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
@@ -1332,7 +1326,7 @@
   <dimension ref="C3:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,7 +1351,7 @@
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1456,10 +1450,7 @@
         <v>230.4</v>
       </c>
       <c r="F10" s="7">
-        <v>227.24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
+        <v>227.18</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
@@ -1547,7 +1538,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1723,8 +1714,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1737,7 +1729,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1913,8 +1905,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1927,7 +1920,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2103,8 +2096,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2117,7 +2111,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C28"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2293,8 +2287,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2307,7 +2302,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2508,7 +2503,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2684,8 +2679,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2698,7 +2694,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2874,8 +2870,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2888,7 +2885,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3064,8 +3061,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3078,7 +3076,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A16:A17"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3254,8 +3252,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3268,7 +3267,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3444,8 +3443,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3458,7 +3458,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3520,7 +3520,7 @@
       </c>
       <c r="G3">
         <f>Table269[[#This Row],[Cumulative Weight (g)]]/$F$8*100</f>
-        <v>1.7597888253409591E-2</v>
+        <v>1.7607183730962234E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="G4">
         <f>Table269[[#This Row],[Cumulative Weight (g)]]/$F$8*100</f>
-        <v>4.8834139903211611</v>
+        <v>4.885993485342019</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="G5">
         <f>Table269[[#This Row],[Cumulative Weight (g)]]/$F$8*100</f>
-        <v>67.426308842938838</v>
+        <v>67.461924465181795</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="B6" s="28">
         <f>((B4-B7)/B3)*100</f>
-        <v>-2.6041666666667653E-2</v>
+        <v>2.6041666666667653E-2</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="G6">
         <f>Table269[[#This Row],[Cumulative Weight (g)]]/$F$8*100</f>
-        <v>99.388473383194011</v>
+        <v>99.44097191654194</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="B7" s="29">
         <f>F8</f>
-        <v>227.3</v>
+        <v>227.18</v>
       </c>
       <c r="D7" t="s">
         <v>37</v>
@@ -3603,11 +3603,11 @@
         <v>6.3E-2</v>
       </c>
       <c r="F7">
-        <v>227.27</v>
+        <v>227.15</v>
       </c>
       <c r="G7">
         <f>Table269[[#This Row],[Cumulative Weight (g)]]/$F$8*100</f>
-        <v>99.98680158380995</v>
+        <v>99.986794612201777</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3625,7 +3625,7 @@
         <v>18</v>
       </c>
       <c r="F8">
-        <v>227.3</v>
+        <v>227.18</v>
       </c>
       <c r="G8">
         <f>Table269[[#This Row],[Cumulative Weight (g)]]/$F$8*100</f>
@@ -3634,8 +3634,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3648,7 +3649,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3824,22 +3825,14 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F077CDA97DB95A4D94653A11DC9C480A" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c380a74f21eee2e8dd8077cfc8b5ceac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a3c60aa5-7cae-452a-8daf-4ebdc4628476" xmlns:ns4="67802ed6-2fef-4885-86f9-c0b162db8b06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6c455adcd6d0abd6f14ef189c43e4d43" ns3:_="" ns4:_="">
     <xsd:import namespace="a3c60aa5-7cae-452a-8daf-4ebdc4628476"/>
@@ -4024,6 +4017,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4031,14 +4033,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC2098FA-2E84-415A-A6A0-57EFA51A6488}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F6241E-6C6D-4A8D-9F88-DCD8F063E983}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4053,6 +4047,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC2098FA-2E84-415A-A6A0-57EFA51A6488}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>